<commit_message>
updated current in Makeffile.  Added 2024-04-30 listfile.  Modified listfiles to use the same header strings that the database uses.  Modified SAPsplit.py so that it assumes all input JSONs are in the same directory, as is produced by unzipping *Jsons.7z.  Added a longer description to SAPsplit.py, describing its dependence on the listfile and the *Jsons.7z input files.
</commit_message>
<xml_diff>
--- a/lists/contributor_lists_2023-12-31.xlsx
+++ b/lists/contributor_lists_2023-12-31.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhasegaw/Dropbox/mark/grants/industry/22novah/distributions/2023-12-31/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhasegaw/Dropbox/mark/projects/split_train_test/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FA1B6C4-6C69-8A4D-901E-6C8585ADFD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4A3EEC-7446-9146-A4F7-1E8241F9D0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{5B09B958-01F4-6F4D-955F-4A39BBE4160E}"/>
   </bookViews>
@@ -908,13 +908,13 @@
     <t>70ba239b-9b51-4789-1096-08db6b8d1576</t>
   </si>
   <si>
-    <t>uuid</t>
-  </si>
-  <si>
-    <t>list</t>
-  </si>
-  <si>
-    <t>block</t>
+    <t>ContributorID</t>
+  </si>
+  <si>
+    <t>List#</t>
+  </si>
+  <si>
+    <t>Block#</t>
   </si>
 </sst>
 </file>
@@ -971,9 +971,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1011,7 +1011,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1117,7 +1117,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1259,7 +1259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1270,7 +1270,7 @@
   <dimension ref="A1:C2321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>